<commit_message>
log out page verification is pending
</commit_message>
<xml_diff>
--- a/demoproject/TestDataSheet.xlsx
+++ b/demoproject/TestDataSheet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Execution</t>
   </si>
@@ -31,6 +31,18 @@
   </si>
   <si>
     <t>TestCaseName</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Macbook pro</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -74,9 +86,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,32 +370,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>